<commit_message>
add resutls for each model
</commit_message>
<xml_diff>
--- a/Insights.xlsx
+++ b/Insights.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,17 +472,77 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>DEF</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>DEG</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>COL_DEG</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>UNCOL_DEG</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>ORACLE</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>MATCH</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>IMPROVEMENT</t>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>MATCH_DEF</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>IMPROVEMENT_DEF</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>MATCH_DEG</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>IMPROVEMENT_DEG</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>MATCH_COL_DEG</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>IMPROVEMENT_COL_DEG</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>MATCH_UNCOL_DEG</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>IMPROVEMENT_UNCOL_DEG</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>MATCH_ORACLE</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>IMPROVEMENT_ORACLE</t>
         </is>
       </c>
     </row>
@@ -501,12 +561,48 @@
         <v>8634</v>
       </c>
       <c r="D2" t="n">
-        <v>8352</v>
+        <v>9379</v>
       </c>
       <c r="E2" t="n">
+        <v>8669</v>
+      </c>
+      <c r="F2" t="n">
+        <v>8634</v>
+      </c>
+      <c r="G2" t="n">
+        <v>9059</v>
+      </c>
+      <c r="H2" t="n">
+        <v>8352</v>
+      </c>
+      <c r="I2" t="n">
+        <v>221</v>
+      </c>
+      <c r="J2" t="n">
+        <v>529</v>
+      </c>
+      <c r="K2" t="n">
+        <v>383</v>
+      </c>
+      <c r="L2" t="n">
+        <v>229</v>
+      </c>
+      <c r="M2" t="n">
+        <v>800</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>294</v>
+      </c>
+      <c r="P2" t="n">
+        <v>406</v>
+      </c>
+      <c r="Q2" t="n">
         <v>562</v>
       </c>
-      <c r="F2" t="n">
+      <c r="R2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -521,12 +617,48 @@
         <v>8634</v>
       </c>
       <c r="D3" t="n">
-        <v>8352</v>
+        <v>9379</v>
       </c>
       <c r="E3" t="n">
+        <v>8669</v>
+      </c>
+      <c r="F3" t="n">
+        <v>8634</v>
+      </c>
+      <c r="G3" t="n">
+        <v>9059</v>
+      </c>
+      <c r="H3" t="n">
+        <v>8352</v>
+      </c>
+      <c r="I3" t="n">
+        <v>221</v>
+      </c>
+      <c r="J3" t="n">
+        <v>529</v>
+      </c>
+      <c r="K3" t="n">
+        <v>383</v>
+      </c>
+      <c r="L3" t="n">
+        <v>229</v>
+      </c>
+      <c r="M3" t="n">
+        <v>800</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>294</v>
+      </c>
+      <c r="P3" t="n">
+        <v>406</v>
+      </c>
+      <c r="Q3" t="n">
         <v>562</v>
       </c>
-      <c r="F3" t="n">
+      <c r="R3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -541,12 +673,48 @@
         <v>8636</v>
       </c>
       <c r="D4" t="n">
-        <v>8352</v>
+        <v>9379</v>
       </c>
       <c r="E4" t="n">
+        <v>8669</v>
+      </c>
+      <c r="F4" t="n">
+        <v>8634</v>
+      </c>
+      <c r="G4" t="n">
+        <v>9059</v>
+      </c>
+      <c r="H4" t="n">
+        <v>8352</v>
+      </c>
+      <c r="I4" t="n">
+        <v>221</v>
+      </c>
+      <c r="J4" t="n">
+        <v>529</v>
+      </c>
+      <c r="K4" t="n">
+        <v>385</v>
+      </c>
+      <c r="L4" t="n">
+        <v>227</v>
+      </c>
+      <c r="M4" t="n">
+        <v>798</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>296</v>
+      </c>
+      <c r="P4" t="n">
+        <v>404</v>
+      </c>
+      <c r="Q4" t="n">
         <v>560</v>
       </c>
-      <c r="F4" t="n">
+      <c r="R4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -561,12 +729,48 @@
         <v>8636</v>
       </c>
       <c r="D5" t="n">
-        <v>8352</v>
+        <v>9379</v>
       </c>
       <c r="E5" t="n">
+        <v>8669</v>
+      </c>
+      <c r="F5" t="n">
+        <v>8634</v>
+      </c>
+      <c r="G5" t="n">
+        <v>9059</v>
+      </c>
+      <c r="H5" t="n">
+        <v>8352</v>
+      </c>
+      <c r="I5" t="n">
+        <v>221</v>
+      </c>
+      <c r="J5" t="n">
+        <v>529</v>
+      </c>
+      <c r="K5" t="n">
+        <v>385</v>
+      </c>
+      <c r="L5" t="n">
+        <v>227</v>
+      </c>
+      <c r="M5" t="n">
+        <v>798</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>296</v>
+      </c>
+      <c r="P5" t="n">
+        <v>404</v>
+      </c>
+      <c r="Q5" t="n">
         <v>560</v>
       </c>
-      <c r="F5" t="n">
+      <c r="R5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -581,12 +785,48 @@
         <v>8667</v>
       </c>
       <c r="D6" t="n">
-        <v>8352</v>
+        <v>9379</v>
       </c>
       <c r="E6" t="n">
+        <v>8669</v>
+      </c>
+      <c r="F6" t="n">
+        <v>8634</v>
+      </c>
+      <c r="G6" t="n">
+        <v>9059</v>
+      </c>
+      <c r="H6" t="n">
+        <v>8352</v>
+      </c>
+      <c r="I6" t="n">
+        <v>223</v>
+      </c>
+      <c r="J6" t="n">
+        <v>511</v>
+      </c>
+      <c r="K6" t="n">
+        <v>798</v>
+      </c>
+      <c r="L6" t="n">
+        <v>2</v>
+      </c>
+      <c r="M6" t="n">
+        <v>385</v>
+      </c>
+      <c r="N6" t="n">
+        <v>188</v>
+      </c>
+      <c r="O6" t="n">
+        <v>317</v>
+      </c>
+      <c r="P6" t="n">
+        <v>384</v>
+      </c>
+      <c r="Q6" t="n">
         <v>529</v>
       </c>
-      <c r="F6" t="n">
+      <c r="R6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -601,12 +841,48 @@
         <v>8671</v>
       </c>
       <c r="D7" t="n">
-        <v>8352</v>
+        <v>9379</v>
       </c>
       <c r="E7" t="n">
+        <v>8669</v>
+      </c>
+      <c r="F7" t="n">
+        <v>8634</v>
+      </c>
+      <c r="G7" t="n">
+        <v>9059</v>
+      </c>
+      <c r="H7" t="n">
+        <v>8352</v>
+      </c>
+      <c r="I7" t="n">
+        <v>227</v>
+      </c>
+      <c r="J7" t="n">
+        <v>508</v>
+      </c>
+      <c r="K7" t="n">
+        <v>796</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" t="n">
+        <v>381</v>
+      </c>
+      <c r="N7" t="n">
+        <v>189</v>
+      </c>
+      <c r="O7" t="n">
+        <v>315</v>
+      </c>
+      <c r="P7" t="n">
+        <v>383</v>
+      </c>
+      <c r="Q7" t="n">
         <v>527</v>
       </c>
-      <c r="F7" t="n">
+      <c r="R7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -625,12 +901,48 @@
         <v>8678</v>
       </c>
       <c r="D8" t="n">
-        <v>8352</v>
+        <v>9379</v>
       </c>
       <c r="E8" t="n">
+        <v>8669</v>
+      </c>
+      <c r="F8" t="n">
+        <v>8634</v>
+      </c>
+      <c r="G8" t="n">
+        <v>9059</v>
+      </c>
+      <c r="H8" t="n">
+        <v>8352</v>
+      </c>
+      <c r="I8" t="n">
+        <v>236</v>
+      </c>
+      <c r="J8" t="n">
+        <v>496</v>
+      </c>
+      <c r="K8" t="n">
+        <v>481</v>
+      </c>
+      <c r="L8" t="n">
+        <v>155</v>
+      </c>
+      <c r="M8" t="n">
+        <v>566</v>
+      </c>
+      <c r="N8" t="n">
+        <v>95</v>
+      </c>
+      <c r="O8" t="n">
+        <v>392</v>
+      </c>
+      <c r="P8" t="n">
+        <v>336</v>
+      </c>
+      <c r="Q8" t="n">
         <v>520</v>
       </c>
-      <c r="F8" t="n">
+      <c r="R8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -645,12 +957,48 @@
         <v>8630</v>
       </c>
       <c r="D9" t="n">
-        <v>8352</v>
+        <v>9379</v>
       </c>
       <c r="E9" t="n">
+        <v>8669</v>
+      </c>
+      <c r="F9" t="n">
+        <v>8634</v>
+      </c>
+      <c r="G9" t="n">
+        <v>9059</v>
+      </c>
+      <c r="H9" t="n">
+        <v>8352</v>
+      </c>
+      <c r="I9" t="n">
+        <v>218</v>
+      </c>
+      <c r="J9" t="n">
+        <v>528</v>
+      </c>
+      <c r="K9" t="n">
+        <v>659</v>
+      </c>
+      <c r="L9" t="n">
+        <v>88</v>
+      </c>
+      <c r="M9" t="n">
+        <v>524</v>
+      </c>
+      <c r="N9" t="n">
+        <v>135</v>
+      </c>
+      <c r="O9" t="n">
+        <v>294</v>
+      </c>
+      <c r="P9" t="n">
+        <v>407</v>
+      </c>
+      <c r="Q9" t="n">
         <v>561</v>
       </c>
-      <c r="F9" t="n">
+      <c r="R9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -665,12 +1013,48 @@
         <v>8616</v>
       </c>
       <c r="D10" t="n">
-        <v>8352</v>
+        <v>9379</v>
       </c>
       <c r="E10" t="n">
+        <v>8669</v>
+      </c>
+      <c r="F10" t="n">
+        <v>8634</v>
+      </c>
+      <c r="G10" t="n">
+        <v>9059</v>
+      </c>
+      <c r="H10" t="n">
+        <v>8352</v>
+      </c>
+      <c r="I10" t="n">
+        <v>216</v>
+      </c>
+      <c r="J10" t="n">
+        <v>533</v>
+      </c>
+      <c r="K10" t="n">
+        <v>517</v>
+      </c>
+      <c r="L10" t="n">
+        <v>166</v>
+      </c>
+      <c r="M10" t="n">
+        <v>666</v>
+      </c>
+      <c r="N10" t="n">
+        <v>71</v>
+      </c>
+      <c r="O10" t="n">
+        <v>277</v>
+      </c>
+      <c r="P10" t="n">
+        <v>423</v>
+      </c>
+      <c r="Q10" t="n">
         <v>573</v>
       </c>
-      <c r="F10" t="n">
+      <c r="R10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -685,12 +1069,48 @@
         <v>8673</v>
       </c>
       <c r="D11" t="n">
-        <v>8352</v>
+        <v>9379</v>
       </c>
       <c r="E11" t="n">
+        <v>8669</v>
+      </c>
+      <c r="F11" t="n">
+        <v>8634</v>
+      </c>
+      <c r="G11" t="n">
+        <v>9059</v>
+      </c>
+      <c r="H11" t="n">
+        <v>8352</v>
+      </c>
+      <c r="I11" t="n">
+        <v>235</v>
+      </c>
+      <c r="J11" t="n">
+        <v>499</v>
+      </c>
+      <c r="K11" t="n">
+        <v>482</v>
+      </c>
+      <c r="L11" t="n">
+        <v>157</v>
+      </c>
+      <c r="M11" t="n">
+        <v>570</v>
+      </c>
+      <c r="N11" t="n">
+        <v>95</v>
+      </c>
+      <c r="O11" t="n">
+        <v>388</v>
+      </c>
+      <c r="P11" t="n">
+        <v>340</v>
+      </c>
+      <c r="Q11" t="n">
         <v>524</v>
       </c>
-      <c r="F11" t="n">
+      <c r="R11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -705,12 +1125,48 @@
         <v>8670</v>
       </c>
       <c r="D12" t="n">
-        <v>8352</v>
+        <v>9379</v>
       </c>
       <c r="E12" t="n">
+        <v>8669</v>
+      </c>
+      <c r="F12" t="n">
+        <v>8634</v>
+      </c>
+      <c r="G12" t="n">
+        <v>9059</v>
+      </c>
+      <c r="H12" t="n">
+        <v>8352</v>
+      </c>
+      <c r="I12" t="n">
+        <v>232</v>
+      </c>
+      <c r="J12" t="n">
+        <v>503</v>
+      </c>
+      <c r="K12" t="n">
+        <v>693</v>
+      </c>
+      <c r="L12" t="n">
+        <v>53</v>
+      </c>
+      <c r="M12" t="n">
+        <v>445</v>
+      </c>
+      <c r="N12" t="n">
+        <v>157</v>
+      </c>
+      <c r="O12" t="n">
+        <v>345</v>
+      </c>
+      <c r="P12" t="n">
+        <v>364</v>
+      </c>
+      <c r="Q12" t="n">
         <v>527</v>
       </c>
-      <c r="F12" t="n">
+      <c r="R12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -725,12 +1181,48 @@
         <v>8701</v>
       </c>
       <c r="D13" t="n">
-        <v>8352</v>
+        <v>9379</v>
       </c>
       <c r="E13" t="n">
+        <v>8669</v>
+      </c>
+      <c r="F13" t="n">
+        <v>8634</v>
+      </c>
+      <c r="G13" t="n">
+        <v>9059</v>
+      </c>
+      <c r="H13" t="n">
+        <v>8352</v>
+      </c>
+      <c r="I13" t="n">
+        <v>236</v>
+      </c>
+      <c r="J13" t="n">
+        <v>489</v>
+      </c>
+      <c r="K13" t="n">
+        <v>613</v>
+      </c>
+      <c r="L13" t="n">
+        <v>79</v>
+      </c>
+      <c r="M13" t="n">
+        <v>434</v>
+      </c>
+      <c r="N13" t="n">
+        <v>151</v>
+      </c>
+      <c r="O13" t="n">
+        <v>405</v>
+      </c>
+      <c r="P13" t="n">
+        <v>320</v>
+      </c>
+      <c r="Q13" t="n">
         <v>505</v>
       </c>
-      <c r="F13" t="n">
+      <c r="R13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -749,12 +1241,48 @@
         <v>8634</v>
       </c>
       <c r="D14" t="n">
-        <v>8352</v>
+        <v>9379</v>
       </c>
       <c r="E14" t="n">
+        <v>8669</v>
+      </c>
+      <c r="F14" t="n">
+        <v>8634</v>
+      </c>
+      <c r="G14" t="n">
+        <v>9059</v>
+      </c>
+      <c r="H14" t="n">
+        <v>8352</v>
+      </c>
+      <c r="I14" t="n">
+        <v>221</v>
+      </c>
+      <c r="J14" t="n">
+        <v>529</v>
+      </c>
+      <c r="K14" t="n">
+        <v>383</v>
+      </c>
+      <c r="L14" t="n">
+        <v>229</v>
+      </c>
+      <c r="M14" t="n">
+        <v>800</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>294</v>
+      </c>
+      <c r="P14" t="n">
+        <v>406</v>
+      </c>
+      <c r="Q14" t="n">
         <v>562</v>
       </c>
-      <c r="F14" t="n">
+      <c r="R14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -769,12 +1297,48 @@
         <v>8634</v>
       </c>
       <c r="D15" t="n">
-        <v>8352</v>
+        <v>9379</v>
       </c>
       <c r="E15" t="n">
+        <v>8669</v>
+      </c>
+      <c r="F15" t="n">
+        <v>8634</v>
+      </c>
+      <c r="G15" t="n">
+        <v>9059</v>
+      </c>
+      <c r="H15" t="n">
+        <v>8352</v>
+      </c>
+      <c r="I15" t="n">
+        <v>221</v>
+      </c>
+      <c r="J15" t="n">
+        <v>529</v>
+      </c>
+      <c r="K15" t="n">
+        <v>383</v>
+      </c>
+      <c r="L15" t="n">
+        <v>229</v>
+      </c>
+      <c r="M15" t="n">
+        <v>800</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>294</v>
+      </c>
+      <c r="P15" t="n">
+        <v>406</v>
+      </c>
+      <c r="Q15" t="n">
         <v>562</v>
       </c>
-      <c r="F15" t="n">
+      <c r="R15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -789,12 +1353,48 @@
         <v>8634</v>
       </c>
       <c r="D16" t="n">
-        <v>8352</v>
+        <v>9379</v>
       </c>
       <c r="E16" t="n">
+        <v>8669</v>
+      </c>
+      <c r="F16" t="n">
+        <v>8634</v>
+      </c>
+      <c r="G16" t="n">
+        <v>9059</v>
+      </c>
+      <c r="H16" t="n">
+        <v>8352</v>
+      </c>
+      <c r="I16" t="n">
+        <v>221</v>
+      </c>
+      <c r="J16" t="n">
+        <v>529</v>
+      </c>
+      <c r="K16" t="n">
+        <v>383</v>
+      </c>
+      <c r="L16" t="n">
+        <v>229</v>
+      </c>
+      <c r="M16" t="n">
+        <v>800</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>294</v>
+      </c>
+      <c r="P16" t="n">
+        <v>406</v>
+      </c>
+      <c r="Q16" t="n">
         <v>562</v>
       </c>
-      <c r="F16" t="n">
+      <c r="R16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -809,12 +1409,48 @@
         <v>8634</v>
       </c>
       <c r="D17" t="n">
-        <v>8352</v>
+        <v>9379</v>
       </c>
       <c r="E17" t="n">
+        <v>8669</v>
+      </c>
+      <c r="F17" t="n">
+        <v>8634</v>
+      </c>
+      <c r="G17" t="n">
+        <v>9059</v>
+      </c>
+      <c r="H17" t="n">
+        <v>8352</v>
+      </c>
+      <c r="I17" t="n">
+        <v>221</v>
+      </c>
+      <c r="J17" t="n">
+        <v>529</v>
+      </c>
+      <c r="K17" t="n">
+        <v>383</v>
+      </c>
+      <c r="L17" t="n">
+        <v>229</v>
+      </c>
+      <c r="M17" t="n">
+        <v>800</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" t="n">
+        <v>294</v>
+      </c>
+      <c r="P17" t="n">
+        <v>406</v>
+      </c>
+      <c r="Q17" t="n">
         <v>562</v>
       </c>
-      <c r="F17" t="n">
+      <c r="R17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -829,12 +1465,48 @@
         <v>8669</v>
       </c>
       <c r="D18" t="n">
-        <v>8352</v>
+        <v>9379</v>
       </c>
       <c r="E18" t="n">
+        <v>8669</v>
+      </c>
+      <c r="F18" t="n">
+        <v>8634</v>
+      </c>
+      <c r="G18" t="n">
+        <v>9059</v>
+      </c>
+      <c r="H18" t="n">
+        <v>8352</v>
+      </c>
+      <c r="I18" t="n">
+        <v>223</v>
+      </c>
+      <c r="J18" t="n">
+        <v>511</v>
+      </c>
+      <c r="K18" t="n">
+        <v>800</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>383</v>
+      </c>
+      <c r="N18" t="n">
+        <v>188</v>
+      </c>
+      <c r="O18" t="n">
+        <v>319</v>
+      </c>
+      <c r="P18" t="n">
+        <v>382</v>
+      </c>
+      <c r="Q18" t="n">
         <v>527</v>
       </c>
-      <c r="F18" t="n">
+      <c r="R18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -849,12 +1521,48 @@
         <v>8669</v>
       </c>
       <c r="D19" t="n">
-        <v>8352</v>
+        <v>9379</v>
       </c>
       <c r="E19" t="n">
+        <v>8669</v>
+      </c>
+      <c r="F19" t="n">
+        <v>8634</v>
+      </c>
+      <c r="G19" t="n">
+        <v>9059</v>
+      </c>
+      <c r="H19" t="n">
+        <v>8352</v>
+      </c>
+      <c r="I19" t="n">
+        <v>223</v>
+      </c>
+      <c r="J19" t="n">
+        <v>511</v>
+      </c>
+      <c r="K19" t="n">
+        <v>800</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" t="n">
+        <v>383</v>
+      </c>
+      <c r="N19" t="n">
+        <v>188</v>
+      </c>
+      <c r="O19" t="n">
+        <v>319</v>
+      </c>
+      <c r="P19" t="n">
+        <v>382</v>
+      </c>
+      <c r="Q19" t="n">
         <v>527</v>
       </c>
-      <c r="F19" t="n">
+      <c r="R19" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>